<commit_message>
Update resources e added CCAR2 coin
</commit_message>
<xml_diff>
--- a/Valores.xlsx
+++ b/Valores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,11 +452,15 @@
           <t>BCOIN</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="C2" t="n">
-        <v>8.390000000000001</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0,89</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4,76</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -465,64 +469,97 @@
           <t>CCAR</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.082</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0,04</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0,22</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>STEP HERO</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.58</v>
+          <t>CCAR2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0,0001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0,0005</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>WIDI</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.6</v>
+          <t>STEP HERO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0,09</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0,48</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WSO</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1</v>
+          <t>WIDI</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0,10</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0,54</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>WSO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0,01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0,07</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Dólar</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5,33</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5,26</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>